<commit_message>
Fix: clears sheet after save
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -447,10 +447,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.23046875" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
@@ -552,38 +552,125 @@
     <row r="6" ht="14.25" customHeight="1" s="2">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>https://store.kawaius.com/products/productdetail/CA901+Ebony+Polish+Digital+Piano/part_number=C11-CA901EP/1772.0.1.1.59003.0.0.0.0?pp=8&amp;</t>
-        </is>
+          <t>https://store.kawaius.com/products/productdetail/CA701+Premium+Satin+Black+Digital+Piano/part_number=C11-CA701SB/1772.0.1.1.59003.0.0.0.0?pp=8&amp;</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>CA701 Premium Satin Black Digital Piano</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>6099</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>4899</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" s="2">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>https://store.kawaius.com/products/productdetail/CA701+Premium+Satin+White+Digital+Piano/part_number=C11-CA701WH/1772.0.1.1.59003.0.0.0.0?s=part_number&amp;part_number_d=ASC&amp;part_number_c=part_number&amp;t=1&amp;i=all&amp;</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>CA701 Premium Satin White Digital Piano</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>6099</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>4899</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1" s="2">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>https://store.kawaius.com/products/productdetail/part_number=C11-CN301SB/1772.0.1.1</t>
-        </is>
+          <t>https://store.kawaius.com/p/mp7se-professional-stage-piano?pp=8</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" s="2">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>https://store.kawaius.com/products/productdetail/CA901+Ebony+Polish+Digital+Piano/part_number=C11-CA901EP/1772.0.1.1.59003.0.0.0.0?pp=8&amp;</t>
-        </is>
+          <t>https://store.kawaius.com/p/es110-black-triple-pedal-bar?pp=8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1" s="2">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>https://kawaius.com/product/gl-10/</t>
-        </is>
+          <t>https://kawaius.com/product/k-200/</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Kawai K-200 Upright Piano</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>8095</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1" s="2">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>https://kawaius.com/product/cn301/</t>
-        </is>
-      </c>
-    </row>
+          <t>https://kawaius.com/product/gl-40/</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Kawai GL-40 Grand Piano</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>38895</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1" s="2">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>https://kawaius.com/product/k-500/</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Kawai K-500 Upright Piano</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>16095</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1" s="2"/>
+    <row r="18" ht="14.25" customHeight="1" s="2"/>
+    <row r="19" ht="14.25" customHeight="1" s="2"/>
+    <row r="21" ht="14.25" customHeight="1" s="2"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>